<commit_message>
Atualização semanal do dashboard (dados ConectaJL)
</commit_message>
<xml_diff>
--- a/progresso.xlsx
+++ b/progresso.xlsx
@@ -853,7 +853,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H14">
-        <v>64.71</v>
+        <v>66.67</v>
       </c>
       <c r="I14">
         <v>38</v>
@@ -1461,13 +1461,13 @@
         <v>Redes TCP/IP 1</v>
       </c>
       <c r="H33">
-        <v>57.14</v>
+        <v>92.31</v>
       </c>
       <c r="I33">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="J33">
-        <v>70</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34">
@@ -1493,7 +1493,7 @@
         <v>Instalação Blindada</v>
       </c>
       <c r="H34">
-        <v>82.5</v>
+        <v>100</v>
       </c>
       <c r="I34">
         <v>95</v>
@@ -1525,7 +1525,7 @@
         <v>Fibra Óptica</v>
       </c>
       <c r="H35">
-        <v>94.12</v>
+        <v>100</v>
       </c>
       <c r="I35">
         <v>114</v>
@@ -2005,7 +2005,7 @@
         <v>Workshop: Segurança em Equipes Técnicas</v>
       </c>
       <c r="H50">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I50">
         <v>2</v>
@@ -2037,7 +2037,7 @@
         <v>Workshop: Gestão de Inadimplência</v>
       </c>
       <c r="H51">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I51">
         <v>33</v>
@@ -2197,7 +2197,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H56">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I56">
         <v>76</v>
@@ -2837,7 +2837,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H76">
-        <v>58.82</v>
+        <v>60.61</v>
       </c>
       <c r="I76">
         <v>36</v>
@@ -2965,7 +2965,7 @@
         <v>Sucesso do Cliente no Suporte</v>
       </c>
       <c r="H80">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I80">
         <v>51</v>
@@ -2997,7 +2997,7 @@
         <v>Workshop: Gestão de Inadimplência</v>
       </c>
       <c r="H81">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I81">
         <v>33</v>
@@ -3029,7 +3029,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H82">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I82">
         <v>76</v>
@@ -3605,7 +3605,7 @@
         <v>Redes TCP/IP 1</v>
       </c>
       <c r="H100">
-        <v>92.86</v>
+        <v>100</v>
       </c>
       <c r="I100">
         <v>98</v>
@@ -3765,7 +3765,7 @@
         <v>Workshop: Segurança em Equipes Técnicas</v>
       </c>
       <c r="H105">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I105">
         <v>2</v>
@@ -4021,7 +4021,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H113">
-        <v>2.94</v>
+        <v>3.03</v>
       </c>
       <c r="I113">
         <v>2</v>
@@ -4661,7 +4661,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H133">
-        <v>58.82</v>
+        <v>60.61</v>
       </c>
       <c r="I133">
         <v>36</v>
@@ -5173,7 +5173,7 @@
         <v>Wi-Fi Premium Residencial</v>
       </c>
       <c r="H149">
-        <v>80.56</v>
+        <v>100</v>
       </c>
       <c r="I149">
         <v>101</v>
@@ -5365,7 +5365,7 @@
         <v>Workshop: Segurança em Equipes Técnicas</v>
       </c>
       <c r="H155">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I155">
         <v>33</v>
@@ -5397,7 +5397,7 @@
         <v>Wi-Fi Premium Residencial</v>
       </c>
       <c r="H156">
-        <v>63.89</v>
+        <v>79.31</v>
       </c>
       <c r="I156">
         <v>66</v>
@@ -5429,7 +5429,7 @@
         <v>Redes TCP/IP 1</v>
       </c>
       <c r="H157">
-        <v>92.86</v>
+        <v>100</v>
       </c>
       <c r="I157">
         <v>108</v>
@@ -5461,7 +5461,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H158">
-        <v>55.88</v>
+        <v>57.58</v>
       </c>
       <c r="I158">
         <v>25</v>
@@ -5557,7 +5557,7 @@
         <v>Instalação Blindada</v>
       </c>
       <c r="H161">
-        <v>82.5</v>
+        <v>100</v>
       </c>
       <c r="I161">
         <v>95</v>
@@ -5909,7 +5909,7 @@
         <v>Fibra Óptica</v>
       </c>
       <c r="H172">
-        <v>94.12</v>
+        <v>100</v>
       </c>
       <c r="I172">
         <v>115</v>
@@ -6037,7 +6037,7 @@
         <v>Workshop: Gestão de Inadimplência</v>
       </c>
       <c r="H176">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I176">
         <v>33</v>
@@ -6453,7 +6453,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H189">
-        <v>58.82</v>
+        <v>60.61</v>
       </c>
       <c r="I189">
         <v>38</v>
@@ -6485,7 +6485,7 @@
         <v>Workshop: Gestão de Inadimplência</v>
       </c>
       <c r="H190">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I190">
         <v>33</v>
@@ -6677,7 +6677,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H196">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I196">
         <v>76</v>
@@ -6965,7 +6965,7 @@
         <v>Workshop: Segurança em Equipes Técnicas</v>
       </c>
       <c r="H205">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I205">
         <v>33</v>
@@ -7221,7 +7221,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H213">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I213">
         <v>79</v>
@@ -7925,7 +7925,7 @@
         <v>Sucesso do Cliente no Suporte</v>
       </c>
       <c r="H235">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I235">
         <v>51</v>
@@ -8053,7 +8053,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H239">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I239">
         <v>77</v>
@@ -8245,7 +8245,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H245">
-        <v>14.71</v>
+        <v>15.15</v>
       </c>
       <c r="I245">
         <v>6</v>
@@ -9365,7 +9365,7 @@
         <v>Workshop: Gestão de Inadimplência</v>
       </c>
       <c r="H280">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I280">
         <v>33</v>
@@ -9685,13 +9685,13 @@
         <v>Supervisão Eficiente - Como Gerenciar a Segurança em Equipes Técnicas</v>
       </c>
       <c r="H290">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I290">
-        <v>0</v>
-      </c>
-      <c r="J290" t="str">
-        <v>Pendente</v>
+        <v>44</v>
+      </c>
+      <c r="J290">
+        <v>70</v>
       </c>
     </row>
     <row r="291">
@@ -9717,10 +9717,10 @@
         <v>Workshop: Sucesso do Cliente no Suporte</v>
       </c>
       <c r="H291">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I291">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="J291" t="str">
         <v>Curso sem prova</v>
@@ -9749,7 +9749,7 @@
         <v>Workshop: Segurança em Equipes Técnicas</v>
       </c>
       <c r="H292">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I292">
         <v>33</v>
@@ -9781,10 +9781,10 @@
         <v>Workshop: Técnico IoT na Prática</v>
       </c>
       <c r="H293">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I293">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="J293" t="str">
         <v>Curso sem prova</v>
@@ -10037,10 +10037,10 @@
         <v>Workshop: Sucesso do Cliente na Venda</v>
       </c>
       <c r="H301">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I301">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="J301" t="str">
         <v>Curso sem prova</v>
@@ -10069,10 +10069,10 @@
         <v>Workshop: MikroTik na Prática</v>
       </c>
       <c r="H302">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I302">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="J302" t="str">
         <v>Curso sem prova</v>
@@ -10101,10 +10101,10 @@
         <v>Workshop: Certificação de Redes GPON e XGS-PON na Prática</v>
       </c>
       <c r="H303">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I303">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="J303" t="str">
         <v>Curso sem prova</v>
@@ -10261,7 +10261,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H308">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I308">
         <v>76</v>
@@ -10293,7 +10293,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H309">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I309">
         <v>76</v>
@@ -11029,13 +11029,13 @@
         <v>Redes TCP/IP Básico</v>
       </c>
       <c r="H332">
-        <v>31.82</v>
+        <v>100</v>
       </c>
       <c r="I332">
-        <v>8</v>
-      </c>
-      <c r="J332" t="str">
-        <v>Pendente</v>
+        <v>64</v>
+      </c>
+      <c r="J332">
+        <v>100</v>
       </c>
     </row>
     <row r="333">
@@ -11061,13 +11061,13 @@
         <v>Redes TCP/IP Básico</v>
       </c>
       <c r="H333">
-        <v>31.82</v>
+        <v>100</v>
       </c>
       <c r="I333">
-        <v>8</v>
-      </c>
-      <c r="J333" t="str">
-        <v>Pendente</v>
+        <v>64</v>
+      </c>
+      <c r="J333">
+        <v>100</v>
       </c>
     </row>
     <row r="334">
@@ -11093,10 +11093,10 @@
         <v>Redes TCP/IP Intermediário</v>
       </c>
       <c r="H334">
-        <v>10.53</v>
+        <v>78.95</v>
       </c>
       <c r="I334">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="J334" t="str">
         <v>Pendente</v>
@@ -11125,10 +11125,10 @@
         <v>Redes TCP/IP Intermediário</v>
       </c>
       <c r="H335">
-        <v>10.53</v>
+        <v>78.95</v>
       </c>
       <c r="I335">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="J335" t="str">
         <v>Pendente</v>
@@ -11157,10 +11157,10 @@
         <v>Redes TCP/IP Intermediário</v>
       </c>
       <c r="H336">
-        <v>10.53</v>
+        <v>78.95</v>
       </c>
       <c r="I336">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="J336" t="str">
         <v>Pendente</v>
@@ -12405,7 +12405,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H375">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I375">
         <v>76</v>
@@ -13141,7 +13141,7 @@
         <v>Workshop: Gestão de Inadimplência</v>
       </c>
       <c r="H398">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I398">
         <v>33</v>
@@ -13461,7 +13461,7 @@
         <v>Sucesso do Cliente no Suporte</v>
       </c>
       <c r="H408">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I408">
         <v>51</v>
@@ -13493,7 +13493,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H409">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I409">
         <v>33</v>
@@ -13557,7 +13557,7 @@
         <v>Criando Clientes Influenciadores</v>
       </c>
       <c r="H411">
-        <v>93.75</v>
+        <v>100</v>
       </c>
       <c r="I411">
         <v>56</v>
@@ -13813,7 +13813,7 @@
         <v>Workshop: Segurança em Equipes Técnicas</v>
       </c>
       <c r="H419">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I419">
         <v>33</v>
@@ -14069,7 +14069,7 @@
         <v>Workshop: Gestão de Inadimplência</v>
       </c>
       <c r="H427">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I427">
         <v>33</v>
@@ -14741,7 +14741,7 @@
         <v>Workshop: Gestão de Inadimplência</v>
       </c>
       <c r="H448">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I448">
         <v>33</v>
@@ -14837,7 +14837,7 @@
         <v>Criando Clientes Influenciadores</v>
       </c>
       <c r="H451">
-        <v>93.75</v>
+        <v>100</v>
       </c>
       <c r="I451">
         <v>57</v>
@@ -15477,7 +15477,7 @@
         <v>Sucesso do Cliente no Suporte</v>
       </c>
       <c r="H471">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I471">
         <v>51</v>
@@ -15701,7 +15701,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H478">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I478">
         <v>76</v>
@@ -15733,7 +15733,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H479">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I479">
         <v>76</v>
@@ -15797,7 +15797,7 @@
         <v>Criando Clientes Influenciadores</v>
       </c>
       <c r="H481">
-        <v>93.75</v>
+        <v>100</v>
       </c>
       <c r="I481">
         <v>57</v>
@@ -16053,7 +16053,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H489">
-        <v>58.82</v>
+        <v>60.61</v>
       </c>
       <c r="I489">
         <v>36</v>
@@ -16565,7 +16565,7 @@
         <v>Sucesso do Cliente no Suporte</v>
       </c>
       <c r="H505">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I505">
         <v>51</v>
@@ -19797,7 +19797,7 @@
         <v>Wi-Fi Premium Residencial</v>
       </c>
       <c r="H606">
-        <v>36.11</v>
+        <v>44.83</v>
       </c>
       <c r="I606">
         <v>24</v>
@@ -20341,7 +20341,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H623">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I623">
         <v>76</v>
@@ -20725,7 +20725,7 @@
         <v>Fibra Óptica</v>
       </c>
       <c r="H635">
-        <v>94.12</v>
+        <v>100</v>
       </c>
       <c r="I635">
         <v>114</v>
@@ -20757,7 +20757,7 @@
         <v>Instalação Blindada</v>
       </c>
       <c r="H636">
-        <v>82.5</v>
+        <v>100</v>
       </c>
       <c r="I636">
         <v>95</v>
@@ -20789,7 +20789,7 @@
         <v>Redes TCP/IP 1</v>
       </c>
       <c r="H637">
-        <v>21.43</v>
+        <v>23.08</v>
       </c>
       <c r="I637">
         <v>17</v>
@@ -21173,7 +21173,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H649">
-        <v>11.76</v>
+        <v>12.12</v>
       </c>
       <c r="I649">
         <v>5</v>
@@ -21717,7 +21717,7 @@
         <v>Fibra Óptica</v>
       </c>
       <c r="H666">
-        <v>29.41</v>
+        <v>31.25</v>
       </c>
       <c r="I666">
         <v>22</v>
@@ -21941,7 +21941,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H673">
-        <v>2.94</v>
+        <v>3.03</v>
       </c>
       <c r="I673">
         <v>2</v>
@@ -22229,7 +22229,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H682">
-        <v>58.82</v>
+        <v>60.61</v>
       </c>
       <c r="I682">
         <v>38</v>
@@ -22549,7 +22549,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H692">
-        <v>26.47</v>
+        <v>27.27</v>
       </c>
       <c r="I692">
         <v>10</v>
@@ -23029,7 +23029,7 @@
         <v>Workshop: Segurança em Equipes Técnicas</v>
       </c>
       <c r="H707">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I707">
         <v>33</v>
@@ -24885,7 +24885,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H765">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I765">
         <v>77</v>
@@ -24917,7 +24917,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H766">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I766">
         <v>77</v>
@@ -26229,7 +26229,7 @@
         <v>Wi-Fi Premium Residencial</v>
       </c>
       <c r="H807">
-        <v>80.56</v>
+        <v>100</v>
       </c>
       <c r="I807">
         <v>102</v>
@@ -26261,7 +26261,7 @@
         <v>Wi-Fi Premium Residencial</v>
       </c>
       <c r="H808">
-        <v>80.56</v>
+        <v>100</v>
       </c>
       <c r="I808">
         <v>102</v>
@@ -26293,7 +26293,7 @@
         <v>Wi-Fi Premium Residencial</v>
       </c>
       <c r="H809">
-        <v>80.56</v>
+        <v>100</v>
       </c>
       <c r="I809">
         <v>102</v>
@@ -26325,7 +26325,7 @@
         <v>Wi-Fi Premium Residencial</v>
       </c>
       <c r="H810">
-        <v>80.56</v>
+        <v>100</v>
       </c>
       <c r="I810">
         <v>102</v>
@@ -26645,7 +26645,7 @@
         <v>Workshop: Gestão de Inadimplência</v>
       </c>
       <c r="H820">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I820">
         <v>33</v>
@@ -28053,7 +28053,7 @@
         <v>Workshop: Segurança em Equipes Técnicas</v>
       </c>
       <c r="H864">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I864">
         <v>33</v>
@@ -28309,7 +28309,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H872">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I872">
         <v>79</v>
@@ -28821,7 +28821,7 @@
         <v>Workshop: Gestão de Inadimplência</v>
       </c>
       <c r="H888">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I888">
         <v>33</v>
@@ -29045,7 +29045,7 @@
         <v>Wi-Fi Premium Residencial</v>
       </c>
       <c r="H895">
-        <v>80.56</v>
+        <v>100</v>
       </c>
       <c r="I895">
         <v>101</v>
@@ -29557,7 +29557,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H911">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I911">
         <v>76</v>
@@ -30581,7 +30581,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H943">
-        <v>58.82</v>
+        <v>60.61</v>
       </c>
       <c r="I943">
         <v>36</v>
@@ -30741,7 +30741,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H948">
-        <v>2.94</v>
+        <v>3.03</v>
       </c>
       <c r="I948">
         <v>2</v>
@@ -31797,7 +31797,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H981">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I981">
         <v>79</v>
@@ -31829,7 +31829,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H982">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I982">
         <v>79</v>
@@ -34805,7 +34805,7 @@
         <v>Workshop: Segurança em Equipes Técnicas</v>
       </c>
       <c r="H1075">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I1075">
         <v>34</v>
@@ -35317,7 +35317,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H1091">
-        <v>76.47</v>
+        <v>78.79</v>
       </c>
       <c r="I1091">
         <v>49</v>
@@ -39477,7 +39477,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H1221">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I1221">
         <v>76</v>
@@ -39605,7 +39605,7 @@
         <v>Workshop: Gestão de Inadimplência</v>
       </c>
       <c r="H1225">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I1225">
         <v>33</v>
@@ -40309,7 +40309,7 @@
         <v>Sucesso do Cliente no Suporte</v>
       </c>
       <c r="H1247">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I1247">
         <v>52</v>
@@ -40469,7 +40469,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H1252">
-        <v>58.82</v>
+        <v>60.61</v>
       </c>
       <c r="I1252">
         <v>39</v>
@@ -40757,7 +40757,7 @@
         <v>Workshop: Segurança em Equipes Técnicas</v>
       </c>
       <c r="H1261">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I1261">
         <v>34</v>
@@ -40821,7 +40821,7 @@
         <v>Criando Clientes Influenciadores</v>
       </c>
       <c r="H1263">
-        <v>93.75</v>
+        <v>100</v>
       </c>
       <c r="I1263">
         <v>57</v>
@@ -41077,7 +41077,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H1271">
-        <v>58.82</v>
+        <v>60.61</v>
       </c>
       <c r="I1271">
         <v>36</v>
@@ -41301,7 +41301,7 @@
         <v>Sucesso do Cliente no Suporte</v>
       </c>
       <c r="H1278">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I1278">
         <v>51</v>
@@ -41557,7 +41557,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H1286">
-        <v>58.82</v>
+        <v>60.61</v>
       </c>
       <c r="I1286">
         <v>36</v>
@@ -41781,7 +41781,7 @@
         <v>Fibra Óptica</v>
       </c>
       <c r="H1293">
-        <v>94.12</v>
+        <v>100</v>
       </c>
       <c r="I1293">
         <v>114</v>
@@ -41973,7 +41973,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H1299">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I1299">
         <v>76</v>
@@ -42005,7 +42005,7 @@
         <v>Instalação Blindada</v>
       </c>
       <c r="H1300">
-        <v>82.5</v>
+        <v>100</v>
       </c>
       <c r="I1300">
         <v>95</v>
@@ -42133,7 +42133,7 @@
         <v>Redes TCP/IP 1</v>
       </c>
       <c r="H1304">
-        <v>92.86</v>
+        <v>100</v>
       </c>
       <c r="I1304">
         <v>108</v>
@@ -42165,7 +42165,7 @@
         <v>Wi-Fi Premium Residencial</v>
       </c>
       <c r="H1305">
-        <v>22.22</v>
+        <v>27.59</v>
       </c>
       <c r="I1305">
         <v>9</v>
@@ -42389,7 +42389,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H1312">
-        <v>2.94</v>
+        <v>3.03</v>
       </c>
       <c r="I1312">
         <v>2</v>
@@ -42901,7 +42901,7 @@
         <v>Sucesso do Cliente no Suporte</v>
       </c>
       <c r="H1328">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I1328">
         <v>51</v>
@@ -42997,7 +42997,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H1331">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I1331">
         <v>76</v>
@@ -43221,7 +43221,7 @@
         <v>Workshop: Gestão de Inadimplência</v>
       </c>
       <c r="H1338">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I1338">
         <v>33</v>
@@ -43637,7 +43637,7 @@
         <v>Sucesso do Cliente no Suporte</v>
       </c>
       <c r="H1351">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I1351">
         <v>51</v>
@@ -43701,7 +43701,7 @@
         <v>Workshop: Gestão de Inadimplência</v>
       </c>
       <c r="H1353">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I1353">
         <v>33</v>
@@ -43797,7 +43797,7 @@
         <v>Criando Clientes Influenciadores</v>
       </c>
       <c r="H1356">
-        <v>93.75</v>
+        <v>100</v>
       </c>
       <c r="I1356">
         <v>57</v>
@@ -44437,7 +44437,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H1376">
-        <v>64.71</v>
+        <v>66.67</v>
       </c>
       <c r="I1376">
         <v>38</v>
@@ -44469,7 +44469,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H1377">
-        <v>64.71</v>
+        <v>66.67</v>
       </c>
       <c r="I1377">
         <v>38</v>
@@ -44565,7 +44565,7 @@
         <v>Workshop: Segurança em Equipes Técnicas</v>
       </c>
       <c r="H1380">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I1380">
         <v>33</v>
@@ -45525,7 +45525,7 @@
         <v>Sucesso do Cliente no Suporte</v>
       </c>
       <c r="H1410">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I1410">
         <v>51</v>
@@ -45557,7 +45557,7 @@
         <v>Sucesso do Cliente no Suporte</v>
       </c>
       <c r="H1411">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I1411">
         <v>51</v>
@@ -45845,7 +45845,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H1420">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I1420">
         <v>76</v>
@@ -45877,7 +45877,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H1421">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I1421">
         <v>76</v>
@@ -46453,7 +46453,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H1439">
-        <v>58.82</v>
+        <v>60.61</v>
       </c>
       <c r="I1439">
         <v>36</v>
@@ -46997,7 +46997,7 @@
         <v>Workshop: Gestão de Inadimplência</v>
       </c>
       <c r="H1456">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I1456">
         <v>33</v>
@@ -47125,7 +47125,7 @@
         <v>Workshop: Segurança em Equipes Técnicas</v>
       </c>
       <c r="H1460">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I1460">
         <v>33</v>
@@ -47573,7 +47573,7 @@
         <v>Atendimento Encantador</v>
       </c>
       <c r="H1474">
-        <v>100</v>
+        <v>103.03</v>
       </c>
       <c r="I1474">
         <v>76</v>
@@ -47669,7 +47669,7 @@
         <v>Wi-Fi Premium Residencial</v>
       </c>
       <c r="H1477">
-        <v>80.56</v>
+        <v>100</v>
       </c>
       <c r="I1477">
         <v>101</v>

</xml_diff>